<commit_message>
Extended test-suite. Corrected row number for add-row! when adding to an empty sheet.
</commit_message>
<xml_diff>
--- a/test/docjure/testdata/datatypes.xlsx
+++ b/test/docjure/testdata/datatypes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>foo</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -58,10 +58,6 @@
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>6/5/1849</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -73,7 +69,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="21">
+  <numFmts count="15">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
     <numFmt numFmtId="166" formatCode="m/d/yy"/>
@@ -87,14 +83,8 @@
     <numFmt numFmtId="174" formatCode="mmmmm\-yy"/>
     <numFmt numFmtId="175" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="176" formatCode="d\-mmm\-yyyy"/>
-    <numFmt numFmtId="178" formatCode="m/d"/>
-    <numFmt numFmtId="179" formatCode="m/d/yy\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="180" formatCode="m/d/yy\ h:mm"/>
-    <numFmt numFmtId="182" formatCode="m/d/yy\ h:mm"/>
-    <numFmt numFmtId="184" formatCode="d\-mmm\-yyyy"/>
-    <numFmt numFmtId="185" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="186" formatCode="d\-mmm\-yyyy"/>
-    <numFmt numFmtId="187" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="177" formatCode="m/d/yy\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="178" formatCode="m/d/yy\ h:mm"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -137,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -159,20 +149,19 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -545,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -613,8 +602,8 @@
       <c r="C4" s="3">
         <v>0.1</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>10</v>
+      <c r="D4" s="5">
+        <v>38717</v>
       </c>
       <c r="E4" s="18">
         <v>6.9444444444444447E-4</v>
@@ -636,8 +625,8 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="D5" s="5">
-        <v>38717</v>
+      <c r="D5" s="6">
+        <v>38718</v>
       </c>
       <c r="E5" s="18">
         <v>4.1666666666666664E-2</v>
@@ -659,8 +648,8 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="D6" s="6">
-        <v>38718</v>
+      <c r="D6" s="7">
+        <v>38719</v>
       </c>
       <c r="E6" s="20">
         <v>1</v>
@@ -673,257 +662,251 @@
       <c r="B7">
         <v>1000</v>
       </c>
-      <c r="D7" s="7">
-        <v>38719</v>
+      <c r="D7" s="8">
+        <v>38720</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="B8">
         <v>1000000</v>
       </c>
-      <c r="D8" s="8">
-        <v>38720</v>
+      <c r="D8" s="9">
+        <v>38721</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="D9" s="9">
-        <v>38721</v>
+      <c r="D9" s="10">
+        <v>38722</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="D10" s="10">
-        <v>38722</v>
+      <c r="D10" s="11">
+        <v>38723</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="D11" s="11">
-        <v>38723</v>
+      <c r="D11" s="12">
+        <v>38724</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="D12" s="12">
-        <v>38724</v>
+      <c r="D12" s="13">
+        <v>38725</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="D13" s="13">
-        <v>38725</v>
+      <c r="D13" s="14">
+        <v>38726</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="D14" s="14">
-        <v>38726</v>
+      <c r="D14" s="15">
+        <v>38727</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="D15" s="15">
-        <v>38727</v>
+      <c r="D15" s="16">
+        <v>38728</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="D16" s="16">
-        <v>38728</v>
+      <c r="D16" s="5">
+        <v>38729</v>
       </c>
     </row>
     <row r="17" spans="4:4">
       <c r="D17" s="5">
-        <v>38729</v>
+        <v>38730</v>
       </c>
     </row>
     <row r="18" spans="4:4">
       <c r="D18" s="5">
-        <v>38730</v>
+        <v>38731</v>
       </c>
     </row>
     <row r="19" spans="4:4">
       <c r="D19" s="5">
-        <v>38731</v>
+        <v>38732</v>
       </c>
     </row>
     <row r="20" spans="4:4">
       <c r="D20" s="5">
-        <v>38732</v>
+        <v>38733</v>
       </c>
     </row>
     <row r="21" spans="4:4">
       <c r="D21" s="5">
-        <v>38733</v>
+        <v>38734</v>
       </c>
     </row>
     <row r="22" spans="4:4">
       <c r="D22" s="5">
-        <v>38734</v>
+        <v>38735</v>
       </c>
     </row>
     <row r="23" spans="4:4">
       <c r="D23" s="5">
-        <v>38735</v>
+        <v>38736</v>
       </c>
     </row>
     <row r="24" spans="4:4">
       <c r="D24" s="5">
-        <v>38736</v>
+        <v>38737</v>
       </c>
     </row>
     <row r="25" spans="4:4">
       <c r="D25" s="5">
-        <v>38737</v>
+        <v>38738</v>
       </c>
     </row>
     <row r="26" spans="4:4">
       <c r="D26" s="5">
-        <v>38738</v>
+        <v>38739</v>
       </c>
     </row>
     <row r="27" spans="4:4">
       <c r="D27" s="5">
-        <v>38739</v>
+        <v>38740</v>
       </c>
     </row>
     <row r="28" spans="4:4">
       <c r="D28" s="5">
-        <v>38740</v>
+        <v>38741</v>
       </c>
     </row>
     <row r="29" spans="4:4">
       <c r="D29" s="5">
-        <v>38741</v>
+        <v>38742</v>
       </c>
     </row>
     <row r="30" spans="4:4">
       <c r="D30" s="5">
-        <v>38742</v>
+        <v>38743</v>
       </c>
     </row>
     <row r="31" spans="4:4">
       <c r="D31" s="5">
-        <v>38743</v>
+        <v>38744</v>
       </c>
     </row>
     <row r="32" spans="4:4">
       <c r="D32" s="5">
-        <v>38744</v>
+        <v>38745</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="5">
-        <v>38745</v>
+        <v>38746</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" s="5">
-        <v>38746</v>
+        <v>38747</v>
       </c>
     </row>
     <row r="35" spans="4:4">
-      <c r="D35" s="5">
-        <v>38747</v>
+      <c r="D35" s="17">
+        <v>38873</v>
       </c>
     </row>
     <row r="36" spans="4:4">
       <c r="D36" s="17">
-        <v>38873</v>
+        <v>16958</v>
       </c>
     </row>
     <row r="37" spans="4:4">
-      <c r="D37" s="17">
-        <v>16958</v>
+      <c r="D37" s="29">
+        <v>37711</v>
       </c>
     </row>
     <row r="38" spans="4:4">
       <c r="D38" s="30">
-        <v>37711</v>
+        <v>37712</v>
       </c>
     </row>
     <row r="39" spans="4:4">
-      <c r="D39" s="31">
-        <v>37712</v>
+      <c r="D39" s="4">
+        <v>37713</v>
       </c>
     </row>
     <row r="40" spans="4:4">
-      <c r="D40" s="4">
-        <v>37713</v>
+      <c r="D40" s="31">
+        <v>37714</v>
       </c>
     </row>
     <row r="41" spans="4:4">
-      <c r="D41" s="32">
-        <v>37714</v>
+      <c r="D41" s="30">
+        <v>37715</v>
       </c>
     </row>
     <row r="42" spans="4:4">
-      <c r="D42" s="31">
-        <v>37715</v>
+      <c r="D42" s="30">
+        <v>37716</v>
       </c>
     </row>
     <row r="43" spans="4:4">
-      <c r="D43" s="31">
-        <v>37716</v>
+      <c r="D43" s="21">
+        <v>37717</v>
       </c>
     </row>
     <row r="44" spans="4:4">
-      <c r="D44" s="21">
-        <v>37717</v>
+      <c r="D44" s="30">
+        <v>37718</v>
       </c>
     </row>
     <row r="45" spans="4:4">
-      <c r="D45" s="31">
-        <v>37718</v>
+      <c r="D45" s="32">
+        <v>37719</v>
       </c>
     </row>
     <row r="46" spans="4:4">
-      <c r="D46" s="33">
-        <v>37719</v>
+      <c r="D46" s="32">
+        <v>37720</v>
       </c>
     </row>
     <row r="47" spans="4:4">
       <c r="D47" s="33">
-        <v>37720</v>
+        <v>37721</v>
       </c>
     </row>
     <row r="48" spans="4:4">
-      <c r="D48" s="34">
-        <v>37721</v>
+      <c r="D48" s="29">
+        <v>37722</v>
       </c>
     </row>
     <row r="49" spans="4:4">
-      <c r="D49" s="30">
-        <v>37722</v>
+      <c r="D49" s="29">
+        <v>37723</v>
       </c>
     </row>
     <row r="50" spans="4:4">
-      <c r="D50" s="30">
-        <v>37723</v>
+      <c r="D50" s="29">
+        <v>37724</v>
       </c>
     </row>
     <row r="51" spans="4:4">
-      <c r="D51" s="30">
-        <v>37724</v>
+      <c r="D51" s="29">
+        <v>37725</v>
       </c>
     </row>
     <row r="52" spans="4:4">
-      <c r="D52" s="30">
-        <v>37725</v>
+      <c r="D52" s="29">
+        <v>37726</v>
       </c>
     </row>
     <row r="53" spans="4:4">
-      <c r="D53" s="30">
-        <v>37726</v>
+      <c r="D53" s="29">
+        <v>37727</v>
       </c>
     </row>
     <row r="54" spans="4:4">
-      <c r="D54" s="30">
-        <v>37727</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4">
-      <c r="D55" s="30">
+      <c r="D54" s="29">
         <v>37728</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>